<commit_message>
Fix fro Kenya and day28 follow-up
</commit_message>
<xml_diff>
--- a/inst/extdata/day28_dict.xlsx
+++ b/inst/extdata/day28_dict.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
   <si>
     <t>old</t>
   </si>
@@ -119,9 +119,6 @@
     <t>hospit_duration</t>
   </si>
   <si>
-    <t>qual_ok</t>
-  </si>
-  <si>
     <t>a1-pid</t>
   </si>
   <si>
@@ -200,9 +197,6 @@
     <t>n1-n1_8</t>
   </si>
   <si>
-    <t>z1-qual</t>
-  </si>
-  <si>
     <t>a1-contact-success</t>
   </si>
   <si>
@@ -237,6 +231,9 @@
   </si>
   <si>
     <t>hospit_day28</t>
+  </si>
+  <si>
+    <t>deidentified</t>
   </si>
 </sst>
 </file>
@@ -593,305 +590,403 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" style="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="4" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" s="4" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="4" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="4" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B31" s="4" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Day7/28 follow-up export with times
</commit_message>
<xml_diff>
--- a/inst/extdata/day28_dict.xlsx
+++ b/inst/extdata/day28_dict.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="71">
   <si>
     <t>old</t>
   </si>
@@ -234,6 +234,9 @@
   </si>
   <si>
     <t>deidentified</t>
+  </si>
+  <si>
+    <t>start</t>
   </si>
 </sst>
 </file>
@@ -590,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -660,332 +663,343 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>31</v>
+      <c r="A6" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>3</v>
+      <c r="C6" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" s="4" t="s">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
       <c r="C13" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>20</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>66</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>68</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35" s="4" t="s">
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36" s="4" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Increase compatibility with India data + Tanzania pilot data
</commit_message>
<xml_diff>
--- a/inst/extdata/day28_dict.xlsx
+++ b/inst/extdata/day28_dict.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="110">
   <si>
     <t>old</t>
   </si>
@@ -342,6 +342,18 @@
   </si>
   <si>
     <t>location_death_day28</t>
+  </si>
+  <si>
+    <t>a1-district</t>
+  </si>
+  <si>
+    <t>district</t>
+  </si>
+  <si>
+    <t>FormVersion</t>
+  </si>
+  <si>
+    <t>form_version</t>
   </si>
 </sst>
 </file>
@@ -716,21 +728,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:XFD40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.58203125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.58203125" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -744,7 +756,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -758,7 +770,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -772,7 +784,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -786,7 +798,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>60</v>
       </c>
@@ -800,7 +812,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>70</v>
       </c>
@@ -814,7 +826,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>31</v>
       </c>
@@ -828,7 +840,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>32</v>
       </c>
@@ -842,424 +854,452 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="7">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D10" s="6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D11" s="6" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D12" s="6" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>37</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
       <c r="C14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D15" s="6" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15" s="3" t="s">
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D16" s="6" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" s="3" t="s">
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D17" s="6" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17" s="3" t="s">
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D18" s="6" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" s="3" t="s">
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D19" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="9" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19" s="9" t="s">
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D20" s="6" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="9" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20" s="9" t="s">
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D21" s="6" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="9" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="B21" s="7">
-        <v>1</v>
-      </c>
-      <c r="C21" s="9" t="s">
+      <c r="B22" s="7">
+        <v>1</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D22" s="10" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="9" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22" s="9" t="s">
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D23" s="6" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23" s="3" t="s">
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D24" s="6" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24" s="3" t="s">
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D25" s="6" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25" s="3" t="s">
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D26" s="6" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26" s="3" t="s">
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D27" s="6" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27" s="3" t="s">
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D28" s="6" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28" s="3" t="s">
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D29" s="6" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="C29" s="3" t="s">
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D30" s="6" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30" s="3" t="s">
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D31" s="6" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31" s="3" t="s">
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D32" s="6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32" s="3" t="s">
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D33" s="6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33" s="3" t="s">
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D34" s="6" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34" s="3" t="s">
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D35" s="6" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35" s="3" t="s">
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="D36" s="6" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-      <c r="C36" s="3" t="s">
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D37" s="6" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37" s="3" t="s">
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D38" s="6" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B38" s="7">
-        <v>1</v>
-      </c>
-      <c r="C38" s="1" t="s">
+      <c r="B39" s="7">
+        <v>1</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D39" s="8" t="s">
         <v>102</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B40" s="7">
+        <v>1</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Day 28 follow-up export and histograms
</commit_message>
<xml_diff>
--- a/inst/extdata/day28_dict.xlsx
+++ b/inst/extdata/day28_dict.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="121">
   <si>
     <t>old</t>
   </si>
@@ -354,32 +354,66 @@
   </si>
   <si>
     <t>form_version</t>
+  </si>
+  <si>
+    <t>is_tanzania</t>
+  </si>
+  <si>
+    <t>is_india</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>a1-fu_type</t>
+  </si>
+  <si>
+    <t>fu_type</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>timestamp</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>nominal</t>
+  </si>
+  <si>
+    <t>character</t>
+  </si>
+  <si>
+    <t>ordinal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -405,6 +439,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -418,41 +464,83 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -728,581 +816,1005 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:XFD40"/>
+    <sheetView tabSelected="1" topLeftCell="C21" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.58203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.58203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.58203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.58203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="6" t="s">
+      <c r="C1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="7">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" s="7">
+        <v>1</v>
+      </c>
+      <c r="F2" s="7">
+        <v>1</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="7">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="7">
+        <v>1</v>
+      </c>
+      <c r="F3" s="7">
+        <v>1</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="7">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1</v>
+      </c>
+      <c r="F4" s="7">
+        <v>1</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B5" s="7">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="E5" s="7">
+        <v>1</v>
+      </c>
+      <c r="F5" s="7">
+        <v>1</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B6" s="7">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D6" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="E6" s="7">
+        <v>1</v>
+      </c>
+      <c r="F6" s="7">
+        <v>1</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="B7" s="7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D7" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="E7" s="7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="7">
+        <v>1</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="B8" s="7">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D8" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="E8" s="7">
+        <v>1</v>
+      </c>
+      <c r="F8" s="7">
+        <v>1</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="B9" s="7">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D9" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="E9" s="7">
+        <v>1</v>
+      </c>
+      <c r="F9" s="7">
+        <v>1</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B9" s="7">
-        <v>1</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="B10" s="12">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D10" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="E10" s="7">
+        <v>1</v>
+      </c>
+      <c r="F10" s="7">
+        <v>1</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="B11" s="7">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D11" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="E11" s="7">
+        <v>1</v>
+      </c>
+      <c r="F11" s="7">
+        <v>1</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="B12" s="7">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D12" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+      <c r="E12" s="7">
+        <v>1</v>
+      </c>
+      <c r="F12" s="7">
+        <v>1</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12" s="3" t="s">
+      <c r="B13" s="7">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D13" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+      <c r="E13" s="7">
+        <v>1</v>
+      </c>
+      <c r="F13" s="7">
+        <v>1</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B13">
+      <c r="B14" s="7">
         <v>0</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D14" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
+      <c r="E14" s="7">
+        <v>1</v>
+      </c>
+      <c r="F14" s="7">
+        <v>1</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B14">
+      <c r="B15" s="7">
         <v>0</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D15" s="4" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+      <c r="E15" s="7">
+        <v>1</v>
+      </c>
+      <c r="F15" s="7">
+        <v>1</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B15">
+      <c r="B16" s="7">
         <v>0</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D16" s="4" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+      <c r="E16" s="7">
+        <v>1</v>
+      </c>
+      <c r="F16" s="7">
+        <v>1</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17" s="7">
+        <v>1</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="E17" s="7">
+        <v>1</v>
+      </c>
+      <c r="F17" s="7">
+        <v>0</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" s="3" t="s">
+      <c r="B18" s="7">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D18" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+      <c r="E18" s="7">
+        <v>1</v>
+      </c>
+      <c r="F18" s="7">
+        <v>1</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17" s="3" t="s">
+      <c r="B19" s="7">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D19" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+      <c r="E19" s="7">
+        <v>1</v>
+      </c>
+      <c r="F19" s="7">
+        <v>1</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" s="3" t="s">
+      <c r="B20" s="7">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D20" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+      <c r="E20" s="7">
+        <v>1</v>
+      </c>
+      <c r="F20" s="7">
+        <v>1</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19" s="3" t="s">
+      <c r="B21" s="7">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D21" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
+      <c r="E21" s="7">
+        <v>1</v>
+      </c>
+      <c r="F21" s="7">
+        <v>1</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20" s="9" t="s">
+      <c r="B22" s="7">
+        <v>1</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D22" s="6" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="9" t="s">
+      <c r="E22" s="7">
+        <v>1</v>
+      </c>
+      <c r="F22" s="7">
+        <v>1</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21" s="9" t="s">
+      <c r="B23" s="7">
+        <v>1</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D23" s="6" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="9" t="s">
+      <c r="E23" s="7">
+        <v>1</v>
+      </c>
+      <c r="F23" s="7">
+        <v>1</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B22" s="7">
-        <v>1</v>
-      </c>
-      <c r="C22" s="9" t="s">
+      <c r="B24" s="12">
+        <v>1</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D24" s="6" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="9" t="s">
+      <c r="E24" s="7">
+        <v>1</v>
+      </c>
+      <c r="F24" s="7">
+        <v>1</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23" s="9" t="s">
+      <c r="B25" s="7">
+        <v>1</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D25" s="6" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
+      <c r="E25" s="7">
+        <v>1</v>
+      </c>
+      <c r="F25" s="7">
+        <v>1</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24" s="3" t="s">
+      <c r="B26" s="7">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D26" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
+      <c r="E26" s="7">
+        <v>1</v>
+      </c>
+      <c r="F26" s="7">
+        <v>1</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25" s="3" t="s">
+      <c r="B27" s="7">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D27" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
+      <c r="E27" s="7">
+        <v>1</v>
+      </c>
+      <c r="F27" s="7">
+        <v>1</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26" s="3" t="s">
+      <c r="B28" s="7">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D28" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
+      <c r="E28" s="7">
+        <v>1</v>
+      </c>
+      <c r="F28" s="7">
+        <v>1</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27" s="3" t="s">
+      <c r="B29" s="7">
+        <v>1</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D29" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
+      <c r="E29" s="7">
+        <v>1</v>
+      </c>
+      <c r="F29" s="7">
+        <v>1</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28" s="3" t="s">
+      <c r="B30" s="7">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D30" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
+      <c r="E30" s="7">
+        <v>1</v>
+      </c>
+      <c r="F30" s="7">
+        <v>1</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="C29" s="3" t="s">
+      <c r="B31" s="7">
+        <v>1</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D31" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
+      <c r="E31" s="7">
+        <v>1</v>
+      </c>
+      <c r="F31" s="7">
+        <v>1</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30" s="3" t="s">
+      <c r="B32" s="7">
+        <v>1</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D32" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
+      <c r="E32" s="7">
+        <v>1</v>
+      </c>
+      <c r="F32" s="7">
+        <v>1</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31" s="3" t="s">
+      <c r="B33" s="7">
+        <v>1</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D33" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
+      <c r="E33" s="7">
+        <v>1</v>
+      </c>
+      <c r="F33" s="7">
+        <v>1</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32" s="3" t="s">
+      <c r="B34" s="7">
+        <v>1</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D34" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
+      <c r="E34" s="7">
+        <v>1</v>
+      </c>
+      <c r="F34" s="7">
+        <v>1</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33" s="3" t="s">
+      <c r="B35" s="7">
+        <v>1</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D35" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
+      <c r="E35" s="7">
+        <v>1</v>
+      </c>
+      <c r="F35" s="7">
+        <v>1</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34" s="3" t="s">
+      <c r="B36" s="7">
+        <v>1</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D36" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
+      <c r="E36" s="7">
+        <v>1</v>
+      </c>
+      <c r="F36" s="7">
+        <v>1</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35" s="3" t="s">
+      <c r="B37" s="7">
+        <v>1</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="D37" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
+      <c r="E37" s="7">
+        <v>1</v>
+      </c>
+      <c r="F37" s="7">
+        <v>1</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-      <c r="C36" s="3" t="s">
+      <c r="B38" s="7">
+        <v>1</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D38" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="3" t="s">
+      <c r="E38" s="7">
+        <v>1</v>
+      </c>
+      <c r="F38" s="7">
+        <v>1</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37" s="3" t="s">
+      <c r="B39" s="7">
+        <v>1</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D39" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
+      <c r="E39" s="7">
+        <v>1</v>
+      </c>
+      <c r="F39" s="7">
+        <v>1</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="C38" s="3" t="s">
+      <c r="B40" s="7">
+        <v>1</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="D40" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
+      <c r="E40" s="7">
+        <v>1</v>
+      </c>
+      <c r="F40" s="7">
+        <v>1</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B39" s="7">
-        <v>1</v>
-      </c>
-      <c r="C39" s="1" t="s">
+      <c r="B41" s="12">
+        <v>1</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D41" s="1" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
+      <c r="E41" s="7">
+        <v>1</v>
+      </c>
+      <c r="F41" s="7">
+        <v>1</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B40" s="7">
-        <v>1</v>
-      </c>
-      <c r="C40" s="1" t="s">
+      <c r="B42" s="12">
+        <v>1</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="D42" s="1" t="s">
         <v>108</v>
       </c>
+      <c r="E42" s="7">
+        <v>1</v>
+      </c>
+      <c r="F42" s="7">
+        <v>1</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>119</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E2:F3 B3 B5:B42 E5:F42">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:F4 B4">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update RCT report and data export
</commit_message>
<xml_diff>
--- a/inst/extdata/day28_dict.xlsx
+++ b/inst/extdata/day28_dict.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="122">
   <si>
     <t>old</t>
   </si>
@@ -387,6 +387,9 @@
   </si>
   <si>
     <t>ordinal</t>
+  </si>
+  <si>
+    <t>stat_analysis</t>
   </si>
 </sst>
 </file>
@@ -509,7 +512,47 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -816,10 +859,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C21" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -831,9 +874,10 @@
     <col min="5" max="5" width="10.25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.08203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -855,8 +899,11 @@
       <c r="G1" s="10" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -878,8 +925,11 @@
       <c r="G2" s="11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>70</v>
       </c>
@@ -901,8 +951,11 @@
       <c r="G3" s="11" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>115</v>
       </c>
@@ -924,8 +977,11 @@
       <c r="G4" s="11" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H4" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -947,8 +1003,11 @@
       <c r="G5" s="11" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -970,8 +1029,11 @@
       <c r="G6" s="11" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>60</v>
       </c>
@@ -993,8 +1055,11 @@
       <c r="G7" s="11" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>31</v>
       </c>
@@ -1016,8 +1081,11 @@
       <c r="G8" s="11" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>32</v>
       </c>
@@ -1039,8 +1107,11 @@
       <c r="G9" s="11" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H9" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>106</v>
       </c>
@@ -1062,8 +1133,11 @@
       <c r="G10" s="11" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>33</v>
       </c>
@@ -1085,8 +1159,11 @@
       <c r="G11" s="11" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H11" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>34</v>
       </c>
@@ -1108,8 +1185,11 @@
       <c r="G12" s="11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H12" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>35</v>
       </c>
@@ -1131,8 +1211,11 @@
       <c r="G13" s="11" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H13" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>36</v>
       </c>
@@ -1154,8 +1237,11 @@
       <c r="G14" s="11" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H14" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>37</v>
       </c>
@@ -1177,8 +1263,11 @@
       <c r="G15" s="11" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H15" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>38</v>
       </c>
@@ -1200,8 +1289,11 @@
       <c r="G16" s="11" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
         <v>113</v>
       </c>
@@ -1223,8 +1315,11 @@
       <c r="G17" s="11" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>57</v>
       </c>
@@ -1246,8 +1341,11 @@
       <c r="G18" s="11" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H18" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>58</v>
       </c>
@@ -1269,8 +1367,11 @@
       <c r="G19" s="11" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H19" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>59</v>
       </c>
@@ -1292,8 +1393,11 @@
       <c r="G20" s="11" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H20" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>10</v>
       </c>
@@ -1315,8 +1419,11 @@
       <c r="G21" s="11" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H21" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>39</v>
       </c>
@@ -1338,8 +1445,11 @@
       <c r="G22" s="11" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H22" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>40</v>
       </c>
@@ -1361,8 +1471,11 @@
       <c r="G23" s="11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H23" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>103</v>
       </c>
@@ -1384,8 +1497,11 @@
       <c r="G24" s="11" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H24" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>41</v>
       </c>
@@ -1407,8 +1523,11 @@
       <c r="G25" s="11" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H25" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>42</v>
       </c>
@@ -1430,8 +1549,11 @@
       <c r="G26" s="11" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H26" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>43</v>
       </c>
@@ -1453,8 +1575,11 @@
       <c r="G27" s="11" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H27" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>44</v>
       </c>
@@ -1476,8 +1601,11 @@
       <c r="G28" s="11" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H28" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>45</v>
       </c>
@@ -1499,8 +1627,11 @@
       <c r="G29" s="11" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H29" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>46</v>
       </c>
@@ -1522,8 +1653,11 @@
       <c r="G30" s="11" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H30" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>47</v>
       </c>
@@ -1545,8 +1679,11 @@
       <c r="G31" s="11" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H31" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>48</v>
       </c>
@@ -1568,8 +1705,11 @@
       <c r="G32" s="11" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H32" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>49</v>
       </c>
@@ -1591,8 +1731,11 @@
       <c r="G33" s="11" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H33" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>50</v>
       </c>
@@ -1614,8 +1757,11 @@
       <c r="G34" s="11" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H34" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>51</v>
       </c>
@@ -1637,8 +1783,11 @@
       <c r="G35" s="11" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H35" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>52</v>
       </c>
@@ -1660,8 +1809,11 @@
       <c r="G36" s="11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H36" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>53</v>
       </c>
@@ -1683,8 +1835,11 @@
       <c r="G37" s="11" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H37" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>54</v>
       </c>
@@ -1706,8 +1861,11 @@
       <c r="G38" s="11" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H38" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>55</v>
       </c>
@@ -1729,8 +1887,11 @@
       <c r="G39" s="11" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H39" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>56</v>
       </c>
@@ -1752,8 +1913,11 @@
       <c r="G40" s="11" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H40" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>100</v>
       </c>
@@ -1775,8 +1939,11 @@
       <c r="G41" s="11" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H41" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>108</v>
       </c>
@@ -1798,19 +1965,123 @@
       <c r="G42" s="11" t="s">
         <v>119</v>
       </c>
+      <c r="H42" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H43" s="7"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H44" s="7"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H45" s="7"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H46" s="7"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H47" s="7"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H48" s="7"/>
+    </row>
+    <row r="49" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H49" s="7"/>
+    </row>
+    <row r="50" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H50" s="7"/>
+    </row>
+    <row r="51" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H51" s="7"/>
+    </row>
+    <row r="52" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H52" s="7"/>
+    </row>
+    <row r="53" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H53" s="7"/>
+    </row>
+    <row r="54" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H54" s="7"/>
+    </row>
+    <row r="55" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H55" s="7"/>
+    </row>
+    <row r="56" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H56" s="7"/>
+    </row>
+    <row r="57" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H57" s="7"/>
+    </row>
+    <row r="58" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H58" s="7"/>
+    </row>
+    <row r="59" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H59" s="7"/>
+    </row>
+    <row r="60" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H60" s="7"/>
+    </row>
+    <row r="61" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H61" s="7"/>
+    </row>
+    <row r="62" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H62" s="7"/>
+    </row>
+    <row r="63" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H63" s="7"/>
+    </row>
+    <row r="64" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H64" s="7"/>
+    </row>
+    <row r="65" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H65" s="7"/>
+    </row>
+    <row r="66" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H66" s="7"/>
+    </row>
+    <row r="67" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H67" s="7"/>
+    </row>
+    <row r="68" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H68" s="7"/>
+    </row>
+    <row r="69" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H69" s="7"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:F3 B3 B5:B42 E5:F42">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:F4 B4">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H42 H44:H47 H50:H69">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H43">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2">
+  <conditionalFormatting sqref="H48">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4:F4 B4">
+  <conditionalFormatting sqref="H49">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
Fix 0 hospitalisation error for India
</commit_message>
<xml_diff>
--- a/inst/extdata/day28_dict.xlsx
+++ b/inst/extdata/day28_dict.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="118">
   <si>
     <t>old</t>
   </si>
@@ -374,19 +374,7 @@
     <t>end</t>
   </si>
   <si>
-    <t>timestamp</t>
-  </si>
-  <si>
-    <t>integer</t>
-  </si>
-  <si>
-    <t>nominal</t>
-  </si>
-  <si>
     <t>character</t>
-  </si>
-  <si>
-    <t>ordinal</t>
   </si>
   <si>
     <t>stat_analysis</t>
@@ -861,8 +849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
-      <selection activeCell="K40" sqref="K40"/>
+    <sheetView tabSelected="1" topLeftCell="C21" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -900,7 +888,7 @@
         <v>112</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -923,7 +911,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>8</v>
+        <v>116</v>
       </c>
       <c r="H2" s="7">
         <v>1</v>
@@ -1001,7 +989,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H5" s="7">
         <v>0</v>
@@ -1027,7 +1015,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H6" s="7">
         <v>0</v>
@@ -1053,7 +1041,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H7" s="7">
         <v>0</v>
@@ -1079,7 +1067,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H8" s="7">
         <v>0</v>
@@ -1105,7 +1093,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H9" s="7">
         <v>1</v>
@@ -1131,7 +1119,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H10" s="7">
         <v>0</v>
@@ -1157,7 +1145,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H11" s="7">
         <v>0</v>
@@ -1183,7 +1171,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>8</v>
+        <v>116</v>
       </c>
       <c r="H12" s="7">
         <v>0</v>
@@ -1209,7 +1197,7 @@
         <v>1</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H13" s="7">
         <v>0</v>
@@ -1235,7 +1223,7 @@
         <v>1</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H14" s="7">
         <v>0</v>
@@ -1261,7 +1249,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H15" s="7">
         <v>0</v>
@@ -1287,7 +1275,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H16" s="7">
         <v>0</v>
@@ -1313,7 +1301,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H17" s="7">
         <v>1</v>
@@ -1339,7 +1327,7 @@
         <v>1</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H18" s="7">
         <v>0</v>
@@ -1365,7 +1353,7 @@
         <v>1</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H19" s="7">
         <v>0</v>
@@ -1391,7 +1379,7 @@
         <v>1</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H20" s="7">
         <v>0</v>
@@ -1417,7 +1405,7 @@
         <v>1</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H21" s="7">
         <v>1</v>
@@ -1443,7 +1431,7 @@
         <v>1</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H22" s="7">
         <v>1</v>
@@ -1469,7 +1457,7 @@
         <v>1</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>8</v>
+        <v>116</v>
       </c>
       <c r="H23" s="7">
         <v>1</v>
@@ -1495,7 +1483,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H24" s="7">
         <v>0</v>
@@ -1521,7 +1509,7 @@
         <v>1</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H25" s="7">
         <v>0</v>
@@ -1547,7 +1535,7 @@
         <v>1</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H26" s="7">
         <v>0</v>
@@ -1573,7 +1561,7 @@
         <v>1</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H27" s="7">
         <v>1</v>
@@ -1599,7 +1587,7 @@
         <v>1</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H28" s="7">
         <v>0</v>
@@ -1625,7 +1613,7 @@
         <v>1</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H29" s="7">
         <v>0</v>
@@ -1651,7 +1639,7 @@
         <v>1</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H30" s="7">
         <v>0</v>
@@ -1677,7 +1665,7 @@
         <v>1</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H31" s="7">
         <v>0</v>
@@ -1703,7 +1691,7 @@
         <v>1</v>
       </c>
       <c r="G32" s="11" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H32" s="7">
         <v>0</v>
@@ -1729,7 +1717,7 @@
         <v>1</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H33" s="7">
         <v>0</v>
@@ -1755,7 +1743,7 @@
         <v>1</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H34" s="7">
         <v>0</v>
@@ -1781,7 +1769,7 @@
         <v>1</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H35" s="7">
         <v>1</v>
@@ -1807,7 +1795,7 @@
         <v>1</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>8</v>
+        <v>116</v>
       </c>
       <c r="H36" s="7">
         <v>1</v>
@@ -1833,7 +1821,7 @@
         <v>1</v>
       </c>
       <c r="G37" s="11" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H37" s="7">
         <v>1</v>
@@ -1859,7 +1847,7 @@
         <v>1</v>
       </c>
       <c r="G38" s="11" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H38" s="7">
         <v>0</v>
@@ -1885,7 +1873,7 @@
         <v>1</v>
       </c>
       <c r="G39" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H39" s="7">
         <v>0</v>
@@ -1911,7 +1899,7 @@
         <v>1</v>
       </c>
       <c r="G40" s="11" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H40" s="7">
         <v>0</v>
@@ -1937,7 +1925,7 @@
         <v>1</v>
       </c>
       <c r="G41" s="11" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H41" s="7">
         <v>1</v>
@@ -1963,7 +1951,7 @@
         <v>1</v>
       </c>
       <c r="G42" s="11" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H42" s="7">
         <v>0</v>

</xml_diff>

<commit_message>
Update Day 7 and Day 28 dictionaries
</commit_message>
<xml_diff>
--- a/inst/extdata/day28_dict.xlsx
+++ b/inst/extdata/day28_dict.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="145">
   <si>
     <t>old</t>
   </si>
@@ -221,9 +221,6 @@
     <t>cure_day28</t>
   </si>
   <si>
-    <t>hf_visit_day28</t>
-  </si>
-  <si>
     <t>date_hosp_day28</t>
   </si>
   <si>
@@ -378,6 +375,90 @@
   </si>
   <si>
     <t>stat_analysis</t>
+  </si>
+  <si>
+    <t>o3_1z</t>
+  </si>
+  <si>
+    <t>hf_visit_day28_no_day7</t>
+  </si>
+  <si>
+    <t>hf_visit_day28_after_day7</t>
+  </si>
+  <si>
+    <t>o3_1aa</t>
+  </si>
+  <si>
+    <t>n1-o3_1aa</t>
+  </si>
+  <si>
+    <t>other_care_yn_no_day7</t>
+  </si>
+  <si>
+    <t>n1-o3_1aaz</t>
+  </si>
+  <si>
+    <t>n1-o3_1z</t>
+  </si>
+  <si>
+    <t>o3_1aaz</t>
+  </si>
+  <si>
+    <t>other_care_yn_after_day7</t>
+  </si>
+  <si>
+    <t>n1-o3_1b</t>
+  </si>
+  <si>
+    <t>other_care_provider</t>
+  </si>
+  <si>
+    <t>o3_1b</t>
+  </si>
+  <si>
+    <t>n1-o3_1b_o</t>
+  </si>
+  <si>
+    <t>o3_1b_o</t>
+  </si>
+  <si>
+    <t>other_care_provider_oth</t>
+  </si>
+  <si>
+    <t>n1-o3_2a</t>
+  </si>
+  <si>
+    <t>o3_2a</t>
+  </si>
+  <si>
+    <t>n1-o3_2b</t>
+  </si>
+  <si>
+    <t>o3_2b</t>
+  </si>
+  <si>
+    <t>n1-o3_2o</t>
+  </si>
+  <si>
+    <t>o3_2o</t>
+  </si>
+  <si>
+    <t>rx_day28</t>
+  </si>
+  <si>
+    <t>rx_day28_oth</t>
+  </si>
+  <si>
+    <t>n1-o3_2az</t>
+  </si>
+  <si>
+    <t>o3_2az</t>
+  </si>
+  <si>
+    <t>rx_day28_yn_no_day7</t>
+  </si>
+  <si>
+    <t>rx_day28_yn_after_day7</t>
   </si>
 </sst>
 </file>
@@ -500,7 +581,187 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="25">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -847,17 +1108,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H69"/>
+  <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C21" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G42"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.58203125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.58203125" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.1640625" bestFit="1" customWidth="1"/>
@@ -870,25 +1131,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E1" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="G1" s="10" t="s">
-        <v>112</v>
-      </c>
       <c r="H1" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -911,7 +1172,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H2" s="7">
         <v>1</v>
@@ -919,16 +1180,16 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" s="7">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E3" s="7">
         <v>1</v>
@@ -937,7 +1198,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H3" s="7">
         <v>1</v>
@@ -945,16 +1206,16 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B4" s="7">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E4" s="7">
         <v>1</v>
@@ -963,7 +1224,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H4" s="7">
         <v>0</v>
@@ -989,7 +1250,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H5" s="7">
         <v>0</v>
@@ -1015,7 +1276,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H6" s="7">
         <v>0</v>
@@ -1041,7 +1302,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H7" s="7">
         <v>0</v>
@@ -1058,7 +1319,7 @@
         <v>3</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E8" s="7">
         <v>1</v>
@@ -1067,7 +1328,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H8" s="7">
         <v>0</v>
@@ -1084,7 +1345,7 @@
         <v>15</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E9" s="7">
         <v>1</v>
@@ -1093,7 +1354,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H9" s="7">
         <v>1</v>
@@ -1101,16 +1362,16 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B10" s="12">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B10" s="12">
-        <v>1</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>107</v>
-      </c>
       <c r="D10" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E10" s="7">
         <v>1</v>
@@ -1119,7 +1380,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H10" s="7">
         <v>0</v>
@@ -1136,7 +1397,7 @@
         <v>16</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E11" s="7">
         <v>1</v>
@@ -1145,7 +1406,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H11" s="7">
         <v>0</v>
@@ -1162,7 +1423,7 @@
         <v>11</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E12" s="7">
         <v>1</v>
@@ -1171,7 +1432,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H12" s="7">
         <v>0</v>
@@ -1188,7 +1449,7 @@
         <v>13</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E13" s="7">
         <v>1</v>
@@ -1197,7 +1458,7 @@
         <v>1</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H13" s="7">
         <v>0</v>
@@ -1223,7 +1484,7 @@
         <v>1</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H14" s="7">
         <v>0</v>
@@ -1240,7 +1501,7 @@
         <v>12</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E15" s="7">
         <v>1</v>
@@ -1249,7 +1510,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H15" s="7">
         <v>0</v>
@@ -1266,7 +1527,7 @@
         <v>14</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E16" s="7">
         <v>1</v>
@@ -1275,7 +1536,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H16" s="7">
         <v>0</v>
@@ -1283,16 +1544,16 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="B17" s="7">
+        <v>1</v>
+      </c>
+      <c r="C17" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="B17" s="7">
-        <v>1</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>114</v>
-      </c>
       <c r="D17" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E17" s="7">
         <v>1</v>
@@ -1301,7 +1562,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H17" s="7">
         <v>1</v>
@@ -1318,7 +1579,7 @@
         <v>17</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E18" s="7">
         <v>1</v>
@@ -1327,7 +1588,7 @@
         <v>1</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H18" s="7">
         <v>0</v>
@@ -1344,7 +1605,7 @@
         <v>19</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E19" s="7">
         <v>1</v>
@@ -1353,7 +1614,7 @@
         <v>1</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H19" s="7">
         <v>0</v>
@@ -1370,7 +1631,7 @@
         <v>18</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E20" s="7">
         <v>1</v>
@@ -1379,7 +1640,7 @@
         <v>1</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H20" s="7">
         <v>0</v>
@@ -1405,7 +1666,7 @@
         <v>1</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H21" s="7">
         <v>1</v>
@@ -1422,7 +1683,7 @@
         <v>62</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E22" s="7">
         <v>1</v>
@@ -1431,7 +1692,7 @@
         <v>1</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H22" s="7">
         <v>1</v>
@@ -1448,7 +1709,7 @@
         <v>63</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E23" s="7">
         <v>1</v>
@@ -1457,7 +1718,7 @@
         <v>1</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H23" s="7">
         <v>1</v>
@@ -1465,17 +1726,17 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B24" s="12">
+        <v>1</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B24" s="12">
-        <v>1</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>104</v>
-      </c>
       <c r="E24" s="7">
         <v>1</v>
       </c>
@@ -1483,7 +1744,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H24" s="7">
         <v>0</v>
@@ -1500,7 +1761,7 @@
         <v>64</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E25" s="7">
         <v>1</v>
@@ -1509,7 +1770,7 @@
         <v>1</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H25" s="7">
         <v>0</v>
@@ -1523,10 +1784,10 @@
         <v>1</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>65</v>
+        <v>118</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E26" s="7">
         <v>1</v>
@@ -1535,7 +1796,7 @@
         <v>1</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H26" s="7">
         <v>0</v>
@@ -1543,16 +1804,16 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>43</v>
+        <v>124</v>
       </c>
       <c r="B27" s="7">
         <v>1</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
       <c r="E27" s="7">
         <v>1</v>
@@ -1561,24 +1822,24 @@
         <v>1</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H27" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B28" s="7">
         <v>1</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E28" s="7">
         <v>1</v>
@@ -1587,24 +1848,24 @@
         <v>1</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H28" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B29" s="7">
         <v>1</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="E29" s="7">
         <v>1</v>
@@ -1613,7 +1874,7 @@
         <v>1</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H29" s="7">
         <v>0</v>
@@ -1621,16 +1882,16 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B30" s="7">
         <v>1</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E30" s="7">
         <v>1</v>
@@ -1639,7 +1900,7 @@
         <v>1</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H30" s="7">
         <v>0</v>
@@ -1647,16 +1908,16 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B31" s="7">
         <v>1</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="E31" s="7">
         <v>1</v>
@@ -1665,7 +1926,7 @@
         <v>1</v>
       </c>
       <c r="G31" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H31" s="7">
         <v>0</v>
@@ -1673,354 +1934,573 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="7">
+        <v>1</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E32" s="7">
+        <v>1</v>
+      </c>
+      <c r="F32" s="7">
+        <v>1</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H32" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B32" s="7">
-        <v>1</v>
-      </c>
-      <c r="C32" s="2" t="s">
+      <c r="B33" s="7">
+        <v>1</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D33" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E33" s="7">
+        <v>1</v>
+      </c>
+      <c r="F33" s="7">
+        <v>1</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H33" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" s="7">
+        <v>1</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E32" s="7">
-        <v>1</v>
-      </c>
-      <c r="F32" s="7">
-        <v>1</v>
-      </c>
-      <c r="G32" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="H32" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B33" s="7">
-        <v>1</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" s="2" t="s">
+      <c r="E34" s="7">
+        <v>1</v>
+      </c>
+      <c r="F34" s="7">
+        <v>1</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H34" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" s="7">
+        <v>1</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E33" s="7">
-        <v>1</v>
-      </c>
-      <c r="F33" s="7">
-        <v>1</v>
-      </c>
-      <c r="G33" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="H33" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B34" s="7">
-        <v>1</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D34" s="2" t="s">
+      <c r="E35" s="7">
+        <v>1</v>
+      </c>
+      <c r="F35" s="7">
+        <v>1</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H35" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" s="7">
+        <v>1</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E36" s="7">
+        <v>1</v>
+      </c>
+      <c r="F36" s="7">
+        <v>1</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H36" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" s="7">
+        <v>1</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E37" s="7">
+        <v>1</v>
+      </c>
+      <c r="F37" s="7">
+        <v>1</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H37" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" s="7">
+        <v>1</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E38" s="7">
+        <v>1</v>
+      </c>
+      <c r="F38" s="7">
+        <v>1</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H38" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39" s="7">
+        <v>1</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E39" s="7">
+        <v>1</v>
+      </c>
+      <c r="F39" s="7">
+        <v>1</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H39" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40" s="7">
+        <v>1</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="E34" s="7">
-        <v>1</v>
-      </c>
-      <c r="F34" s="7">
-        <v>1</v>
-      </c>
-      <c r="G34" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="H34" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B35" s="7">
-        <v>1</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E35" s="7">
-        <v>1</v>
-      </c>
-      <c r="F35" s="7">
-        <v>1</v>
-      </c>
-      <c r="G35" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="H35" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B36" s="7">
-        <v>1</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E36" s="7">
-        <v>1</v>
-      </c>
-      <c r="F36" s="7">
-        <v>1</v>
-      </c>
-      <c r="G36" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="H36" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B37" s="7">
-        <v>1</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E37" s="7">
-        <v>1</v>
-      </c>
-      <c r="F37" s="7">
-        <v>1</v>
-      </c>
-      <c r="G37" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="H37" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B38" s="7">
-        <v>1</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D38" s="2" t="s">
+      <c r="E40" s="7">
+        <v>1</v>
+      </c>
+      <c r="F40" s="7">
+        <v>1</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H40" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B41" s="7">
+        <v>1</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E38" s="7">
-        <v>1</v>
-      </c>
-      <c r="F38" s="7">
-        <v>1</v>
-      </c>
-      <c r="G38" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="H38" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B39" s="7">
-        <v>1</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E39" s="7">
-        <v>1</v>
-      </c>
-      <c r="F39" s="7">
-        <v>1</v>
-      </c>
-      <c r="G39" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="H39" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B40" s="7">
-        <v>1</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E40" s="7">
-        <v>1</v>
-      </c>
-      <c r="F40" s="7">
-        <v>1</v>
-      </c>
-      <c r="G40" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="H40" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
+      <c r="E41" s="7">
+        <v>1</v>
+      </c>
+      <c r="F41" s="7">
+        <v>1</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H41" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="B42" s="7">
+        <v>1</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="E42" s="7">
+        <v>1</v>
+      </c>
+      <c r="F42" s="7">
+        <v>1</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H42" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="B43" s="7">
+        <v>1</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="E43" s="7">
+        <v>1</v>
+      </c>
+      <c r="F43" s="7">
+        <v>1</v>
+      </c>
+      <c r="G43" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H43" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="B44" s="5">
+        <v>1</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D44" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="E44" s="7">
+        <v>1</v>
+      </c>
+      <c r="F44" s="7">
+        <v>1</v>
+      </c>
+      <c r="G44" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H44" s="7">
+        <v>0</v>
+      </c>
+      <c r="I44" s="11"/>
+      <c r="J44" s="7"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="B45" s="5">
+        <v>1</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="E45" s="7">
+        <v>1</v>
+      </c>
+      <c r="F45" s="7">
+        <v>1</v>
+      </c>
+      <c r="G45" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H45" s="7">
+        <v>0</v>
+      </c>
+      <c r="I45" s="11"/>
+      <c r="J45" s="7"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="B46" s="5">
+        <v>1</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E46" s="7">
+        <v>1</v>
+      </c>
+      <c r="F46" s="7">
+        <v>1</v>
+      </c>
+      <c r="G46" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H46" s="7">
+        <v>0</v>
+      </c>
+      <c r="I46" s="11"/>
+      <c r="J46" s="7"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B47" s="5">
+        <v>1</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="E47" s="7">
+        <v>1</v>
+      </c>
+      <c r="F47" s="7">
+        <v>1</v>
+      </c>
+      <c r="G47" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H47" s="7">
+        <v>0</v>
+      </c>
+      <c r="I47" s="11"/>
+      <c r="J47" s="7"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="B48" s="5">
+        <v>1</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="D48" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="E48" s="7">
+        <v>1</v>
+      </c>
+      <c r="F48" s="7">
+        <v>1</v>
+      </c>
+      <c r="G48" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H48" s="7">
+        <v>0</v>
+      </c>
+      <c r="I48" s="11"/>
+      <c r="J48" s="7"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B49" s="5">
+        <v>1</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="D49" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="E49" s="7">
+        <v>1</v>
+      </c>
+      <c r="F49" s="7">
+        <v>1</v>
+      </c>
+      <c r="G49" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H49" s="7">
+        <v>0</v>
+      </c>
+      <c r="I49" s="11"/>
+      <c r="J49" s="7"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B50" s="12">
+        <v>1</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B41" s="12">
-        <v>1</v>
-      </c>
-      <c r="C41" s="1" t="s">
+      <c r="D50" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E41" s="7">
-        <v>1</v>
-      </c>
-      <c r="F41" s="7">
-        <v>1</v>
-      </c>
-      <c r="G41" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="H41" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
+      <c r="E50" s="7">
+        <v>1</v>
+      </c>
+      <c r="F50" s="7">
+        <v>1</v>
+      </c>
+      <c r="G50" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H50" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B51" s="12">
+        <v>1</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B42" s="12">
-        <v>1</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E42" s="7">
-        <v>1</v>
-      </c>
-      <c r="F42" s="7">
-        <v>1</v>
-      </c>
-      <c r="G42" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="H42" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H43" s="7"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H44" s="7"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H45" s="7"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H46" s="7"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H47" s="7"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H48" s="7"/>
-    </row>
-    <row r="49" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H49" s="7"/>
-    </row>
-    <row r="50" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H50" s="7"/>
-    </row>
-    <row r="51" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H51" s="7"/>
-    </row>
-    <row r="52" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="D51" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E51" s="7">
+        <v>1</v>
+      </c>
+      <c r="F51" s="7">
+        <v>1</v>
+      </c>
+      <c r="G51" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H51" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H52" s="7"/>
     </row>
-    <row r="53" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H53" s="7"/>
     </row>
-    <row r="54" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H54" s="7"/>
     </row>
-    <row r="55" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H55" s="7"/>
     </row>
-    <row r="56" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H56" s="7"/>
     </row>
-    <row r="57" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H57" s="7"/>
     </row>
-    <row r="58" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H58" s="7"/>
     </row>
-    <row r="59" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H59" s="7"/>
     </row>
-    <row r="60" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H60" s="7"/>
     </row>
-    <row r="61" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H61" s="7"/>
     </row>
-    <row r="62" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H62" s="7"/>
     </row>
-    <row r="63" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H63" s="7"/>
     </row>
-    <row r="64" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H64" s="7"/>
     </row>
     <row r="65" spans="8:8" x14ac:dyDescent="0.3">
@@ -2038,39 +2518,146 @@
     <row r="69" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H69" s="7"/>
     </row>
+    <row r="70" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H70" s="7"/>
+    </row>
+    <row r="71" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H71" s="7"/>
+    </row>
+    <row r="72" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H72" s="7"/>
+    </row>
+    <row r="73" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H73" s="7"/>
+    </row>
+    <row r="74" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H74" s="7"/>
+    </row>
+    <row r="75" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H75" s="7"/>
+    </row>
+    <row r="76" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H76" s="7"/>
+    </row>
+    <row r="77" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H77" s="7"/>
+    </row>
+    <row r="78" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H78" s="7"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:F3 B3 B5:B42 E5:F42">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+  <conditionalFormatting sqref="E2:F3 B3 B5:B26 E5:F26 E28:F41 B28:B41 B50:B51 E50:F51">
+    <cfRule type="cellIs" dxfId="24" priority="23" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:F4 B4">
+    <cfRule type="cellIs" dxfId="22" priority="21" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H26 H53:H56 H59:H78 H28:H41 H50:H51">
+    <cfRule type="cellIs" dxfId="21" priority="20" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H52">
+    <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H57">
+    <cfRule type="cellIs" dxfId="19" priority="18" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H58">
+    <cfRule type="cellIs" dxfId="18" priority="17" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27 E27:F27">
+    <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H27">
+    <cfRule type="cellIs" dxfId="16" priority="15" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E42:F42 B42">
+    <cfRule type="cellIs" dxfId="15" priority="14" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H42">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E43:F43 B43">
+    <cfRule type="cellIs" dxfId="13" priority="12" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H43:H44">
+    <cfRule type="cellIs" dxfId="12" priority="11" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J44">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J45">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B44 E44:F44">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J46 J48:J49">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H45:H46 H48:H49">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B45 E45:F45">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B46 E46:F46 E48:F49 B48:B49">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H42 H44:H47 H50:H69">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+  <conditionalFormatting sqref="J47">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H43">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+  <conditionalFormatting sqref="H47">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H48">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H49">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="B47 E47:F47">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Various updates following feedback from Kenya
</commit_message>
<xml_diff>
--- a/inst/extdata/day28_dict.xlsx
+++ b/inst/extdata/day28_dict.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="147">
   <si>
     <t>old</t>
   </si>
@@ -459,6 +459,12 @@
   </si>
   <si>
     <t>rx_day28_yn_after_day7</t>
+  </si>
+  <si>
+    <t>SubmissionDate</t>
+  </si>
+  <si>
+    <t>submission_date</t>
   </si>
 </sst>
 </file>
@@ -1108,10 +1114,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J78"/>
+  <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1309,17 +1315,17 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="7">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>71</v>
+      <c r="A8" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="E8" s="7">
         <v>1</v>
@@ -1336,16 +1342,16 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="7">
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E9" s="7">
         <v>1</v>
@@ -1357,21 +1363,21 @@
         <v>115</v>
       </c>
       <c r="H9" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B10" s="12">
+        <v>32</v>
+      </c>
+      <c r="B10" s="7">
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>106</v>
+        <v>15</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
       <c r="E10" s="7">
         <v>1</v>
@@ -1383,21 +1389,21 @@
         <v>115</v>
       </c>
       <c r="H10" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="7">
+        <v>105</v>
+      </c>
+      <c r="B11" s="12">
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>16</v>
+        <v>106</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>73</v>
+        <v>106</v>
       </c>
       <c r="E11" s="7">
         <v>1</v>
@@ -1414,16 +1420,16 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" s="7">
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E12" s="7">
         <v>1</v>
@@ -1440,42 +1446,42 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="7">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="7">
+        <v>1</v>
+      </c>
+      <c r="F13" s="7">
+        <v>1</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H13" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="7">
-        <v>1</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="B14" s="7">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="E13" s="7">
-        <v>1</v>
-      </c>
-      <c r="F13" s="7">
-        <v>1</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H13" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="7">
-        <v>0</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>2</v>
       </c>
       <c r="E14" s="7">
         <v>1</v>
@@ -1492,16 +1498,16 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="7">
         <v>0</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>76</v>
+        <v>2</v>
       </c>
       <c r="E15" s="7">
         <v>1</v>
@@ -1518,94 +1524,94 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="7">
+        <v>0</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="7">
+        <v>1</v>
+      </c>
+      <c r="F16" s="7">
+        <v>1</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H16" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="7">
-        <v>0</v>
-      </c>
-      <c r="C16" s="4" t="s">
+      <c r="B17" s="7">
+        <v>0</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="E16" s="7">
-        <v>1</v>
-      </c>
-      <c r="F16" s="7">
-        <v>1</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H16" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="13" t="s">
+      <c r="E17" s="7">
+        <v>1</v>
+      </c>
+      <c r="F17" s="7">
+        <v>1</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H17" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="B17" s="7">
-        <v>1</v>
-      </c>
-      <c r="C17" s="13" t="s">
+      <c r="B18" s="7">
+        <v>1</v>
+      </c>
+      <c r="C18" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D18" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="E17" s="7">
-        <v>1</v>
-      </c>
-      <c r="F17" s="7">
-        <v>0</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H17" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B18" s="7">
-        <v>1</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="E18" s="7">
         <v>1</v>
       </c>
       <c r="F18" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18" s="11" t="s">
         <v>115</v>
       </c>
       <c r="H18" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B19" s="7">
         <v>1</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="E19" s="7">
         <v>1</v>
@@ -1622,16 +1628,16 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B20" s="7">
         <v>1</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E20" s="7">
         <v>1</v>
@@ -1648,42 +1654,42 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="7">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E21" s="7">
+        <v>1</v>
+      </c>
+      <c r="F21" s="7">
+        <v>1</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H21" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="7">
-        <v>1</v>
-      </c>
-      <c r="C21" s="2" t="s">
+      <c r="B22" s="7">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="E21" s="7">
-        <v>1</v>
-      </c>
-      <c r="F21" s="7">
-        <v>1</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H21" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="7">
-        <v>1</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>93</v>
       </c>
       <c r="E22" s="7">
         <v>1</v>
@@ -1700,16 +1706,16 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B23" s="7">
         <v>1</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="E23" s="7">
         <v>1</v>
@@ -1726,16 +1732,16 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="B24" s="12">
+        <v>40</v>
+      </c>
+      <c r="B24" s="7">
         <v>1</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>104</v>
+        <v>63</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="E24" s="7">
         <v>1</v>
@@ -1747,47 +1753,47 @@
         <v>115</v>
       </c>
       <c r="H24" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B25" s="12">
+        <v>1</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E25" s="7">
+        <v>1</v>
+      </c>
+      <c r="F25" s="7">
+        <v>1</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H25" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="7">
-        <v>1</v>
-      </c>
-      <c r="C25" s="6" t="s">
+      <c r="B26" s="7">
+        <v>1</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D26" s="6" t="s">
         <v>80</v>
-      </c>
-      <c r="E25" s="7">
-        <v>1</v>
-      </c>
-      <c r="F25" s="7">
-        <v>1</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H25" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B26" s="7">
-        <v>1</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="E26" s="7">
         <v>1</v>
@@ -1804,16 +1810,16 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>124</v>
+        <v>42</v>
       </c>
       <c r="B27" s="7">
         <v>1</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>117</v>
+        <v>81</v>
       </c>
       <c r="E27" s="7">
         <v>1</v>
@@ -1830,16 +1836,16 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>43</v>
+        <v>124</v>
       </c>
       <c r="B28" s="7">
         <v>1</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>94</v>
+        <v>117</v>
       </c>
       <c r="E28" s="7">
         <v>1</v>
@@ -1851,21 +1857,21 @@
         <v>115</v>
       </c>
       <c r="H28" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B29" s="7">
         <v>1</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E29" s="7">
         <v>1</v>
@@ -1877,21 +1883,21 @@
         <v>115</v>
       </c>
       <c r="H29" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B30" s="7">
         <v>1</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="E30" s="7">
         <v>1</v>
@@ -1908,16 +1914,16 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B31" s="7">
         <v>1</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E31" s="7">
         <v>1</v>
@@ -1934,16 +1940,16 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B32" s="7">
         <v>1</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E32" s="7">
         <v>1</v>
@@ -1960,16 +1966,16 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B33" s="7">
         <v>1</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="E33" s="7">
         <v>1</v>
@@ -1986,16 +1992,16 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B34" s="7">
         <v>1</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E34" s="7">
         <v>1</v>
@@ -2012,16 +2018,16 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B35" s="7">
         <v>1</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E35" s="7">
         <v>1</v>
@@ -2038,16 +2044,16 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B36" s="7">
         <v>1</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="E36" s="7">
         <v>1</v>
@@ -2059,21 +2065,21 @@
         <v>115</v>
       </c>
       <c r="H36" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B37" s="7">
         <v>1</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>65</v>
+        <v>27</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E37" s="7">
         <v>1</v>
@@ -2090,16 +2096,16 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B38" s="7">
         <v>1</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E38" s="7">
         <v>1</v>
@@ -2116,16 +2122,16 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B39" s="7">
         <v>1</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E39" s="7">
         <v>1</v>
@@ -2137,21 +2143,21 @@
         <v>115</v>
       </c>
       <c r="H39" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B40" s="7">
         <v>1</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>67</v>
+        <v>28</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E40" s="7">
         <v>1</v>
@@ -2168,42 +2174,42 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41" s="7">
+        <v>1</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E41" s="7">
+        <v>1</v>
+      </c>
+      <c r="F41" s="7">
+        <v>1</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H41" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="7">
-        <v>1</v>
-      </c>
-      <c r="C41" s="2" t="s">
+      <c r="B42" s="7">
+        <v>1</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="E41" s="7">
-        <v>1</v>
-      </c>
-      <c r="F41" s="7">
-        <v>1</v>
-      </c>
-      <c r="G41" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H41" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A42" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="B42" s="7">
-        <v>1</v>
-      </c>
-      <c r="C42" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="D42" s="13" t="s">
-        <v>120</v>
       </c>
       <c r="E42" s="7">
         <v>1</v>
@@ -2220,16 +2226,16 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="13" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B43" s="7">
         <v>1</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E43" s="7">
         <v>1</v>
@@ -2246,16 +2252,16 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="B44" s="5">
+        <v>123</v>
+      </c>
+      <c r="B44" s="7">
         <v>1</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D44" s="13" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E44" s="7">
         <v>1</v>
@@ -2269,21 +2275,19 @@
       <c r="H44" s="7">
         <v>0</v>
       </c>
-      <c r="I44" s="11"/>
-      <c r="J44" s="7"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B45" s="5">
         <v>1</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D45" s="13" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E45" s="7">
         <v>1</v>
@@ -2302,16 +2306,16 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="13" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B46" s="5">
         <v>1</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E46" s="7">
         <v>1</v>
@@ -2330,16 +2334,16 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="13" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="B47" s="5">
         <v>1</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D47" s="13" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="E47" s="7">
         <v>1</v>
@@ -2358,16 +2362,16 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="13" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="B48" s="5">
         <v>1</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="D48" s="13" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E48" s="7">
         <v>1</v>
@@ -2386,16 +2390,16 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="13" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B49" s="5">
         <v>1</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D49" s="13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E49" s="7">
         <v>1</v>
@@ -2413,17 +2417,17 @@
       <c r="J49" s="7"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B50" s="12">
-        <v>1</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>101</v>
+      <c r="A50" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B50" s="5">
+        <v>1</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="D50" s="13" t="s">
+        <v>138</v>
       </c>
       <c r="E50" s="7">
         <v>1</v>
@@ -2435,37 +2439,62 @@
         <v>115</v>
       </c>
       <c r="H50" s="7">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I50" s="11"/>
+      <c r="J50" s="7"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B51" s="12">
+        <v>1</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E51" s="7">
+        <v>1</v>
+      </c>
+      <c r="F51" s="7">
+        <v>1</v>
+      </c>
+      <c r="G51" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H51" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B51" s="12">
-        <v>1</v>
-      </c>
-      <c r="C51" s="1" t="s">
+      <c r="B52" s="12">
+        <v>1</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D52" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E51" s="7">
-        <v>1</v>
-      </c>
-      <c r="F51" s="7">
-        <v>1</v>
-      </c>
-      <c r="G51" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H51" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H52" s="7"/>
+      <c r="E52" s="7">
+        <v>1</v>
+      </c>
+      <c r="F52" s="7">
+        <v>1</v>
+      </c>
+      <c r="G52" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H52" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H53" s="7"/>
@@ -2545,119 +2574,132 @@
     <row r="78" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H78" s="7"/>
     </row>
+    <row r="79" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H79" s="7"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:F3 B3 B5:B26 E5:F26 E28:F41 B28:B41 B50:B51 E50:F51">
-    <cfRule type="cellIs" dxfId="24" priority="23" operator="equal">
+  <conditionalFormatting sqref="E2:F3 B3 B5:B7 E5:F7 E29:F42 B29:B42 B51:B52 E51:F52 E9:F27 B9:B27">
+    <cfRule type="cellIs" dxfId="24" priority="27" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="26" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:F4 B4">
-    <cfRule type="cellIs" dxfId="22" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="25" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H26 H53:H56 H59:H78 H28:H41 H50:H51">
-    <cfRule type="cellIs" dxfId="21" priority="20" operator="equal">
+  <conditionalFormatting sqref="H2:H7 H54:H57 H60:H79 H29:H42 H51:H52 H9:H27">
+    <cfRule type="cellIs" dxfId="21" priority="24" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H52">
-    <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H57">
-    <cfRule type="cellIs" dxfId="19" priority="18" operator="equal">
+  <conditionalFormatting sqref="H53">
+    <cfRule type="cellIs" dxfId="20" priority="23" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H58">
-    <cfRule type="cellIs" dxfId="18" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="22" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B27 E27:F27">
-    <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
+  <conditionalFormatting sqref="H59">
+    <cfRule type="cellIs" dxfId="18" priority="21" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H27">
-    <cfRule type="cellIs" dxfId="16" priority="15" operator="equal">
+  <conditionalFormatting sqref="B28 E28:F28">
+    <cfRule type="cellIs" dxfId="17" priority="20" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E42:F42 B42">
-    <cfRule type="cellIs" dxfId="15" priority="14" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H42">
-    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+  <conditionalFormatting sqref="H28">
+    <cfRule type="cellIs" dxfId="16" priority="19" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43:F43 B43">
-    <cfRule type="cellIs" dxfId="13" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="18" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H43:H44">
-    <cfRule type="cellIs" dxfId="12" priority="11" operator="equal">
+  <conditionalFormatting sqref="H43">
+    <cfRule type="cellIs" dxfId="14" priority="17" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J44">
-    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+  <conditionalFormatting sqref="E44:F44 B44">
+    <cfRule type="cellIs" dxfId="13" priority="16" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H44:H45">
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J45">
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B44 E44:F44">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J46 J48:J49">
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H45:H46 H48:H49">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+  <conditionalFormatting sqref="J46">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45 E45:F45">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="14" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B46 E46:F46 E48:F49 B48:B49">
+  <conditionalFormatting sqref="J47 J49:J50">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H46:H47 H49:H50">
+    <cfRule type="cellIs" dxfId="7" priority="12" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B46 E46:F46">
+    <cfRule type="cellIs" dxfId="6" priority="11" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B47 E47:F47 E49:F50 B49:B50">
+    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J48">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J47">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+  <conditionalFormatting sqref="H48">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H47">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+  <conditionalFormatting sqref="B48 E48:F48">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B47 E47:F47">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+  <conditionalFormatting sqref="B8">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8:F8 H8">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update to fix Senegal and Tanzania
</commit_message>
<xml_diff>
--- a/inst/extdata/day28_dict.xlsx
+++ b/inst/extdata/day28_dict.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="145">
   <si>
     <t>old</t>
   </si>
@@ -359,9 +359,6 @@
     <t>is_india</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
     <t>a1-fu_type</t>
   </si>
   <si>
@@ -369,9 +366,6 @@
   </si>
   <si>
     <t>end</t>
-  </si>
-  <si>
-    <t>character</t>
   </si>
   <si>
     <t>stat_analysis</t>
@@ -542,7 +536,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -570,9 +564,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1114,10 +1105,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J79"/>
+  <dimension ref="A1:I79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1128,11 +1119,10 @@
     <col min="4" max="4" width="15.58203125" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.08203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1151,14 +1141,11 @@
       <c r="F1" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="G1" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G1" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -1177,14 +1164,11 @@
       <c r="F2" s="7">
         <v>1</v>
       </c>
-      <c r="G2" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H2" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G2" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>69</v>
       </c>
@@ -1203,25 +1187,22 @@
       <c r="F3" s="7">
         <v>1</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H3" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G3" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B4" s="7">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E4" s="7">
         <v>1</v>
@@ -1229,14 +1210,11 @@
       <c r="F4" s="7">
         <v>1</v>
       </c>
-      <c r="G4" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H4" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G4" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1255,14 +1233,11 @@
       <c r="F5" s="7">
         <v>1</v>
       </c>
-      <c r="G5" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H5" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G5" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1281,14 +1256,11 @@
       <c r="F6" s="7">
         <v>1</v>
       </c>
-      <c r="G6" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H6" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G6" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>60</v>
       </c>
@@ -1307,25 +1279,22 @@
       <c r="F7" s="7">
         <v>1</v>
       </c>
-      <c r="G7" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H7" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G7" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B8" s="5">
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E8" s="7">
         <v>1</v>
@@ -1333,14 +1302,11 @@
       <c r="F8" s="7">
         <v>1</v>
       </c>
-      <c r="G8" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H8" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G8" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>31</v>
       </c>
@@ -1359,14 +1325,11 @@
       <c r="F9" s="7">
         <v>1</v>
       </c>
-      <c r="G9" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H9" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G9" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>32</v>
       </c>
@@ -1385,18 +1348,15 @@
       <c r="F10" s="7">
         <v>1</v>
       </c>
-      <c r="G10" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H10" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G10" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="11">
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -1411,14 +1371,11 @@
       <c r="F11" s="7">
         <v>1</v>
       </c>
-      <c r="G11" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H11" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G11" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>33</v>
       </c>
@@ -1437,14 +1394,11 @@
       <c r="F12" s="7">
         <v>1</v>
       </c>
-      <c r="G12" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H12" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G12" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>34</v>
       </c>
@@ -1463,14 +1417,11 @@
       <c r="F13" s="7">
         <v>1</v>
       </c>
-      <c r="G13" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H13" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G13" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>35</v>
       </c>
@@ -1489,14 +1440,11 @@
       <c r="F14" s="7">
         <v>1</v>
       </c>
-      <c r="G14" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H14" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G14" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>36</v>
       </c>
@@ -1515,14 +1463,11 @@
       <c r="F15" s="7">
         <v>1</v>
       </c>
-      <c r="G15" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H15" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G15" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>37</v>
       </c>
@@ -1541,14 +1486,11 @@
       <c r="F16" s="7">
         <v>1</v>
       </c>
-      <c r="G16" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H16" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G16" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>38</v>
       </c>
@@ -1567,25 +1509,22 @@
       <c r="F17" s="7">
         <v>1</v>
       </c>
-      <c r="G17" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H17" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="13" t="s">
+      <c r="G17" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B18" s="7">
+        <v>1</v>
+      </c>
+      <c r="C18" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="B18" s="7">
-        <v>1</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>113</v>
+      <c r="D18" s="12" t="s">
+        <v>112</v>
       </c>
       <c r="E18" s="7">
         <v>1</v>
@@ -1593,14 +1532,11 @@
       <c r="F18" s="7">
         <v>0</v>
       </c>
-      <c r="G18" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H18" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G18" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>57</v>
       </c>
@@ -1619,14 +1555,11 @@
       <c r="F19" s="7">
         <v>1</v>
       </c>
-      <c r="G19" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H19" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G19" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>58</v>
       </c>
@@ -1645,14 +1578,11 @@
       <c r="F20" s="7">
         <v>1</v>
       </c>
-      <c r="G20" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H20" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G20" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>59</v>
       </c>
@@ -1671,14 +1601,11 @@
       <c r="F21" s="7">
         <v>1</v>
       </c>
-      <c r="G21" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H21" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G21" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>10</v>
       </c>
@@ -1697,14 +1624,11 @@
       <c r="F22" s="7">
         <v>1</v>
       </c>
-      <c r="G22" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H22" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G22" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>39</v>
       </c>
@@ -1723,14 +1647,11 @@
       <c r="F23" s="7">
         <v>1</v>
       </c>
-      <c r="G23" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H23" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G23" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>40</v>
       </c>
@@ -1749,18 +1670,15 @@
       <c r="F24" s="7">
         <v>1</v>
       </c>
-      <c r="G24" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H24" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G24" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B25" s="12">
+      <c r="B25" s="11">
         <v>1</v>
       </c>
       <c r="C25" s="6" t="s">
@@ -1775,14 +1693,11 @@
       <c r="F25" s="7">
         <v>1</v>
       </c>
-      <c r="G25" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H25" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G25" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>41</v>
       </c>
@@ -1801,14 +1716,11 @@
       <c r="F26" s="7">
         <v>1</v>
       </c>
-      <c r="G26" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H26" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G26" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>42</v>
       </c>
@@ -1816,7 +1728,7 @@
         <v>1</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>81</v>
@@ -1827,40 +1739,34 @@
       <c r="F27" s="7">
         <v>1</v>
       </c>
-      <c r="G27" s="11" t="s">
+      <c r="G27" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B28" s="7">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="H27" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B28" s="7">
-        <v>1</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>117</v>
-      </c>
       <c r="E28" s="7">
         <v>1</v>
       </c>
       <c r="F28" s="7">
         <v>1</v>
       </c>
-      <c r="G28" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H28" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G28" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>43</v>
       </c>
@@ -1879,14 +1785,11 @@
       <c r="F29" s="7">
         <v>1</v>
       </c>
-      <c r="G29" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H29" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G29" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>44</v>
       </c>
@@ -1905,14 +1808,11 @@
       <c r="F30" s="7">
         <v>1</v>
       </c>
-      <c r="G30" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H30" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G30" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>45</v>
       </c>
@@ -1931,14 +1831,11 @@
       <c r="F31" s="7">
         <v>1</v>
       </c>
-      <c r="G31" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H31" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G31" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>46</v>
       </c>
@@ -1957,14 +1854,11 @@
       <c r="F32" s="7">
         <v>1</v>
       </c>
-      <c r="G32" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H32" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G32" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>47</v>
       </c>
@@ -1983,14 +1877,11 @@
       <c r="F33" s="7">
         <v>1</v>
       </c>
-      <c r="G33" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H33" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G33" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>48</v>
       </c>
@@ -2009,14 +1900,11 @@
       <c r="F34" s="7">
         <v>1</v>
       </c>
-      <c r="G34" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H34" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G34" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>49</v>
       </c>
@@ -2035,14 +1923,11 @@
       <c r="F35" s="7">
         <v>1</v>
       </c>
-      <c r="G35" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H35" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G35" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>50</v>
       </c>
@@ -2061,14 +1946,11 @@
       <c r="F36" s="7">
         <v>1</v>
       </c>
-      <c r="G36" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H36" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G36" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>51</v>
       </c>
@@ -2087,14 +1969,11 @@
       <c r="F37" s="7">
         <v>1</v>
       </c>
-      <c r="G37" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H37" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G37" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>52</v>
       </c>
@@ -2113,14 +1992,11 @@
       <c r="F38" s="7">
         <v>1</v>
       </c>
-      <c r="G38" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H38" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G38" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>53</v>
       </c>
@@ -2139,14 +2015,11 @@
       <c r="F39" s="7">
         <v>1</v>
       </c>
-      <c r="G39" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H39" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G39" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>54</v>
       </c>
@@ -2165,14 +2038,11 @@
       <c r="F40" s="7">
         <v>1</v>
       </c>
-      <c r="G40" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H40" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G40" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>55</v>
       </c>
@@ -2191,14 +2061,11 @@
       <c r="F41" s="7">
         <v>1</v>
       </c>
-      <c r="G41" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H41" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G41" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>56</v>
       </c>
@@ -2217,238 +2084,211 @@
       <c r="F42" s="7">
         <v>1</v>
       </c>
-      <c r="G42" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H42" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43" s="13" t="s">
+      <c r="G42" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B43" s="7">
+        <v>1</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="E43" s="7">
+        <v>1</v>
+      </c>
+      <c r="F43" s="7">
+        <v>1</v>
+      </c>
+      <c r="G43" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="B43" s="7">
-        <v>1</v>
-      </c>
-      <c r="C43" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="D43" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="E43" s="7">
-        <v>1</v>
-      </c>
-      <c r="F43" s="7">
-        <v>1</v>
-      </c>
-      <c r="G43" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H43" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A44" s="13" t="s">
+      <c r="B44" s="7">
+        <v>1</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="D44" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="B44" s="7">
-        <v>1</v>
-      </c>
-      <c r="C44" s="13" t="s">
+      <c r="E44" s="7">
+        <v>1</v>
+      </c>
+      <c r="F44" s="7">
+        <v>1</v>
+      </c>
+      <c r="G44" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B45" s="5">
+        <v>1</v>
+      </c>
+      <c r="C45" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="D44" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="E44" s="7">
-        <v>1</v>
-      </c>
-      <c r="F44" s="7">
-        <v>1</v>
-      </c>
-      <c r="G44" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H44" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45" s="13" t="s">
+      <c r="D45" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="B45" s="5">
-        <v>1</v>
-      </c>
-      <c r="C45" s="13" t="s">
+      <c r="E45" s="7">
+        <v>1</v>
+      </c>
+      <c r="F45" s="7">
+        <v>1</v>
+      </c>
+      <c r="G45" s="7">
+        <v>0</v>
+      </c>
+      <c r="H45" s="10"/>
+      <c r="I45" s="7"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="D45" s="13" t="s">
+      <c r="B46" s="5">
+        <v>1</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="D46" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="E45" s="7">
-        <v>1</v>
-      </c>
-      <c r="F45" s="7">
-        <v>1</v>
-      </c>
-      <c r="G45" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H45" s="7">
-        <v>0</v>
-      </c>
-      <c r="I45" s="11"/>
-      <c r="J45" s="7"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="B46" s="5">
-        <v>1</v>
-      </c>
-      <c r="C46" s="13" t="s">
+      <c r="E46" s="7">
+        <v>1</v>
+      </c>
+      <c r="F46" s="7">
+        <v>1</v>
+      </c>
+      <c r="G46" s="7">
+        <v>0</v>
+      </c>
+      <c r="H46" s="10"/>
+      <c r="I46" s="7"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B47" s="5">
+        <v>1</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="D47" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="D46" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="E46" s="7">
-        <v>1</v>
-      </c>
-      <c r="F46" s="7">
-        <v>1</v>
-      </c>
-      <c r="G46" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H46" s="7">
-        <v>0</v>
-      </c>
-      <c r="I46" s="11"/>
-      <c r="J46" s="7"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A47" s="13" t="s">
+      <c r="E47" s="7">
+        <v>1</v>
+      </c>
+      <c r="F47" s="7">
+        <v>1</v>
+      </c>
+      <c r="G47" s="7">
+        <v>0</v>
+      </c>
+      <c r="H47" s="10"/>
+      <c r="I47" s="7"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="B48" s="5">
+        <v>1</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="E48" s="7">
+        <v>1</v>
+      </c>
+      <c r="F48" s="7">
+        <v>1</v>
+      </c>
+      <c r="G48" s="7">
+        <v>0</v>
+      </c>
+      <c r="H48" s="10"/>
+      <c r="I48" s="7"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="B47" s="5">
-        <v>1</v>
-      </c>
-      <c r="C47" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="D47" s="13" t="s">
+      <c r="B49" s="5">
+        <v>1</v>
+      </c>
+      <c r="C49" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="D49" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="E47" s="7">
-        <v>1</v>
-      </c>
-      <c r="F47" s="7">
-        <v>1</v>
-      </c>
-      <c r="G47" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H47" s="7">
-        <v>0</v>
-      </c>
-      <c r="I47" s="11"/>
-      <c r="J47" s="7"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A48" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="B48" s="5">
-        <v>1</v>
-      </c>
-      <c r="C48" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="D48" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="E48" s="7">
-        <v>1</v>
-      </c>
-      <c r="F48" s="7">
-        <v>1</v>
-      </c>
-      <c r="G48" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H48" s="7">
-        <v>0</v>
-      </c>
-      <c r="I48" s="11"/>
-      <c r="J48" s="7"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A49" s="13" t="s">
+      <c r="E49" s="7">
+        <v>1</v>
+      </c>
+      <c r="F49" s="7">
+        <v>1</v>
+      </c>
+      <c r="G49" s="7">
+        <v>0</v>
+      </c>
+      <c r="H49" s="10"/>
+      <c r="I49" s="7"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="B49" s="5">
-        <v>1</v>
-      </c>
-      <c r="C49" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="D49" s="13" t="s">
+      <c r="B50" s="5">
+        <v>1</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="D50" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="E49" s="7">
-        <v>1</v>
-      </c>
-      <c r="F49" s="7">
-        <v>1</v>
-      </c>
-      <c r="G49" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H49" s="7">
-        <v>0</v>
-      </c>
-      <c r="I49" s="11"/>
-      <c r="J49" s="7"/>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A50" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="B50" s="5">
-        <v>1</v>
-      </c>
-      <c r="C50" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="D50" s="13" t="s">
-        <v>138</v>
-      </c>
       <c r="E50" s="7">
         <v>1</v>
       </c>
       <c r="F50" s="7">
         <v>1</v>
       </c>
-      <c r="G50" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H50" s="7">
-        <v>0</v>
-      </c>
-      <c r="I50" s="11"/>
-      <c r="J50" s="7"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G50" s="7">
+        <v>0</v>
+      </c>
+      <c r="H50" s="10"/>
+      <c r="I50" s="7"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B51" s="12">
+      <c r="B51" s="11">
         <v>1</v>
       </c>
       <c r="C51" s="1" t="s">
@@ -2463,18 +2303,15 @@
       <c r="F51" s="7">
         <v>1</v>
       </c>
-      <c r="G51" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H51" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G51" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B52" s="12">
+      <c r="B52" s="11">
         <v>1</v>
       </c>
       <c r="C52" s="1" t="s">
@@ -2489,93 +2326,90 @@
       <c r="F52" s="7">
         <v>1</v>
       </c>
-      <c r="G52" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="H52" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H53" s="7"/>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H54" s="7"/>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H55" s="7"/>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H56" s="7"/>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H57" s="7"/>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H58" s="7"/>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H59" s="7"/>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H60" s="7"/>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H61" s="7"/>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H62" s="7"/>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H63" s="7"/>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H64" s="7"/>
-    </row>
-    <row r="65" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H65" s="7"/>
-    </row>
-    <row r="66" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H66" s="7"/>
-    </row>
-    <row r="67" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H67" s="7"/>
-    </row>
-    <row r="68" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H68" s="7"/>
-    </row>
-    <row r="69" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H69" s="7"/>
-    </row>
-    <row r="70" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H70" s="7"/>
-    </row>
-    <row r="71" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H71" s="7"/>
-    </row>
-    <row r="72" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H72" s="7"/>
-    </row>
-    <row r="73" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H73" s="7"/>
-    </row>
-    <row r="74" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H74" s="7"/>
-    </row>
-    <row r="75" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H75" s="7"/>
-    </row>
-    <row r="76" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H76" s="7"/>
-    </row>
-    <row r="77" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H77" s="7"/>
-    </row>
-    <row r="78" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H78" s="7"/>
-    </row>
-    <row r="79" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H79" s="7"/>
+      <c r="G52" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G53" s="7"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G54" s="7"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G55" s="7"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G56" s="7"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G57" s="7"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G58" s="7"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G59" s="7"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G60" s="7"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G61" s="7"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G62" s="7"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G63" s="7"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G64" s="7"/>
+    </row>
+    <row r="65" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G65" s="7"/>
+    </row>
+    <row r="66" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G66" s="7"/>
+    </row>
+    <row r="67" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G67" s="7"/>
+    </row>
+    <row r="68" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G68" s="7"/>
+    </row>
+    <row r="69" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G69" s="7"/>
+    </row>
+    <row r="70" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G70" s="7"/>
+    </row>
+    <row r="71" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G71" s="7"/>
+    </row>
+    <row r="72" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G72" s="7"/>
+    </row>
+    <row r="73" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G73" s="7"/>
+    </row>
+    <row r="74" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G74" s="7"/>
+    </row>
+    <row r="75" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G75" s="7"/>
+    </row>
+    <row r="76" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G76" s="7"/>
+    </row>
+    <row r="77" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G77" s="7"/>
+    </row>
+    <row r="78" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G78" s="7"/>
+    </row>
+    <row r="79" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G79" s="7"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:F3 B3 B5:B7 E5:F7 E29:F42 B29:B42 B51:B52 E51:F52 E9:F27 B9:B27">
@@ -2593,22 +2427,22 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H7 H54:H57 H60:H79 H29:H42 H51:H52 H9:H27">
+  <conditionalFormatting sqref="G2:G7 G54:G57 G60:G79 G29:G42 G51:G52 G9:G27">
     <cfRule type="cellIs" dxfId="21" priority="24" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H53">
+  <conditionalFormatting sqref="G53">
     <cfRule type="cellIs" dxfId="20" priority="23" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H58">
+  <conditionalFormatting sqref="G58">
     <cfRule type="cellIs" dxfId="19" priority="22" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H59">
+  <conditionalFormatting sqref="G59">
     <cfRule type="cellIs" dxfId="18" priority="21" operator="equal">
       <formula>1</formula>
     </cfRule>
@@ -2618,7 +2452,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H28">
+  <conditionalFormatting sqref="G28">
     <cfRule type="cellIs" dxfId="16" priority="19" operator="equal">
       <formula>1</formula>
     </cfRule>
@@ -2628,7 +2462,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H43">
+  <conditionalFormatting sqref="G43">
     <cfRule type="cellIs" dxfId="14" priority="17" operator="equal">
       <formula>1</formula>
     </cfRule>
@@ -2638,17 +2472,17 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H44:H45">
+  <conditionalFormatting sqref="G44:G45">
     <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J45">
+  <conditionalFormatting sqref="I45">
     <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J46">
+  <conditionalFormatting sqref="I46">
     <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
       <formula>1</formula>
     </cfRule>
@@ -2658,12 +2492,12 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J47 J49:J50">
+  <conditionalFormatting sqref="I47 I49:I50">
     <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H46:H47 H49:H50">
+  <conditionalFormatting sqref="G46:G47 G49:G50">
     <cfRule type="cellIs" dxfId="7" priority="12" operator="equal">
       <formula>1</formula>
     </cfRule>
@@ -2678,12 +2512,12 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J48">
+  <conditionalFormatting sqref="I48">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H48">
+  <conditionalFormatting sqref="G48">
     <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
       <formula>1</formula>
     </cfRule>
@@ -2698,7 +2532,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E8:F8 H8">
+  <conditionalFormatting sqref="E8:G8">
     <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>

</xml_diff>

<commit_message>
Hard lock for Senegal
</commit_message>
<xml_diff>
--- a/inst/extdata/day28_dict.xlsx
+++ b/inst/extdata/day28_dict.xlsx
@@ -1105,7 +1105,7 @@
   <dimension ref="A1:I79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1193,7 +1193,7 @@
         <v>112</v>
       </c>
       <c r="B4" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>112</v>
@@ -1216,7 +1216,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>7</v>
@@ -1262,7 +1262,7 @@
         <v>59</v>
       </c>
       <c r="B7" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>9</v>
@@ -1285,7 +1285,7 @@
         <v>142</v>
       </c>
       <c r="B8" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>143</v>

</xml_diff>